<commit_message>
added macro support to schema-util
</commit_message>
<xml_diff>
--- a/node-js/schema-util/cardlist.xlsx
+++ b/node-js/schema-util/cardlist.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TriAdX\Documents\Volition-Git\node-js\schema-util\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/git/cryptogogue/volition/node-js/schema-util/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A57569B-6861-4910-82DE-16DA3F338D4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="510" windowWidth="22830" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4220" yWindow="860" windowWidth="31620" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
+    <sheet name="macros" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -310,12 +310,39 @@
   </si>
   <si>
     <t>Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it.Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it.Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it.Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it.Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it. Enter - You may pick a depleted dude and inflict 1 damage to it.</t>
+  </si>
+  <si>
+    <t>FOOP</t>
+  </si>
+  <si>
+    <t>DOOP</t>
+  </si>
+  <si>
+    <t>BLOOP</t>
+  </si>
+  <si>
+    <t>foop</t>
+  </si>
+  <si>
+    <t>&lt;$b&gt;doop&lt;$&gt;</t>
+  </si>
+  <si>
+    <t>bloop bloop bloop</t>
+  </si>
+  <si>
+    <t>Arty {{ DOOP }}</t>
+  </si>
+  <si>
+    <t>{{ FOOP }} McArtison</t>
+  </si>
+  <si>
+    <t>Arty {{ BLOOP }} McArtison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,38 +688,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="29" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="1"/>
+    <col min="19" max="19" width="14.1640625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
@@ -742,7 +769,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>69</v>
       </c>
@@ -792,7 +819,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -907,7 +934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -966,7 +993,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -1025,7 +1052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="42" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -1084,7 +1111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -1143,7 +1170,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>14</v>
       </c>
@@ -1202,7 +1229,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>16</v>
       </c>
@@ -1246,7 +1273,7 @@
         <v>51</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>31</v>
@@ -1261,7 +1288,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>18</v>
       </c>
@@ -1305,7 +1332,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>31</v>
@@ -1320,7 +1347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>21</v>
       </c>
@@ -1364,7 +1391,7 @@
         <v>53</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>31</v>
@@ -1383,4 +1410,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated font paths to use git repo
</commit_message>
<xml_diff>
--- a/node-js/schema-util/cardlist.xlsx
+++ b/node-js/schema-util/cardlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18340" yWindow="3620" windowWidth="21440" windowHeight="11120"/>
+    <workbookView xWindow="9980" yWindow="6760" windowWidth="21440" windowHeight="11120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4343" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4343" uniqueCount="820">
   <si>
     <t>Name</t>
   </si>
@@ -2384,18 +2384,6 @@
   </si>
   <si>
     <t>roboto</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/fonts/roboto/roboto-regular.ttf</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/fonts/roboto/roboto-bold.ttf</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/fonts/roboto/roboto-regularitalic.ttf</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/fonts/roboto/roboto-bolditalic.ttf</t>
   </si>
   <si>
     <t>ICONS</t>
@@ -3175,12 +3163,15 @@
   <si>
     <t>DEFINITIONS</t>
   </si>
+  <si>
+    <t>https://cors-anywhere.herokuapp.com/https://github.com/cryptogogue/vol-cardmotron-js-assets/blob/master/fonts/roboto/Roboto-Regular.ttf?raw=true</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3220,6 +3211,14 @@
       <color theme="0"/>
       <name val="VolitionFont"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3263,10 +3262,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3372,8 +3372,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3678,7 +3682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3758,7 +3762,7 @@
     </row>
     <row r="6" spans="1:22" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B6" s="40"/>
       <c r="C6" s="39" t="s">
@@ -5719,8 +5723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5764,17 +5768,17 @@
       <c r="C2" s="15" t="s">
         <v>699</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>700</v>
+      <c r="D2" s="43" t="s">
+        <v>819</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>701</v>
+        <v>819</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>702</v>
+        <v>819</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>703</v>
+        <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5782,26 +5786,26 @@
     </row>
     <row r="4" spans="1:7" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="13"/>
       <c r="C5" s="15" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D5" s="11">
         <v>256</v>
@@ -5810,14 +5814,14 @@
         <v>256</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="15" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="D6" s="11">
         <v>1</v>
@@ -5826,14 +5830,14 @@
         <v>1</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="15" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D7" s="11">
         <v>650</v>
@@ -5842,14 +5846,14 @@
         <v>450</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="13"/>
       <c r="C8" s="15" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D8" s="11">
         <v>650</v>
@@ -5858,14 +5862,14 @@
         <v>450</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="15" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D9" s="11">
         <v>650</v>
@@ -5874,14 +5878,14 @@
         <v>450</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13"/>
       <c r="C10" s="15" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D10" s="11">
         <v>650</v>
@@ -5890,14 +5894,14 @@
         <v>450</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
       <c r="C11" s="15" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D11" s="11">
         <v>650</v>
@@ -5906,14 +5910,14 @@
         <v>450</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="15" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D12" s="11">
         <v>650</v>
@@ -5922,14 +5926,14 @@
         <v>450</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="13"/>
       <c r="C13" s="15" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="D13" s="11">
         <v>650</v>
@@ -5938,14 +5942,14 @@
         <v>450</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="13"/>
       <c r="C14" s="15" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D14" s="11">
         <v>650</v>
@@ -5954,14 +5958,14 @@
         <v>450</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="C15" s="15" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="D15" s="11">
         <v>650</v>
@@ -5970,14 +5974,14 @@
         <v>450</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13"/>
       <c r="C16" s="15" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D16" s="11">
         <v>650</v>
@@ -5986,14 +5990,14 @@
         <v>450</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13"/>
       <c r="C17" s="15" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D17" s="11">
         <v>650</v>
@@ -6002,70 +6006,70 @@
         <v>450</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="G17" s="5"/>
     </row>
     <row r="19" spans="1:18" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>733</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>735</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>736</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>707</v>
-      </c>
-      <c r="G19" s="14" t="s">
+      <c r="M19" s="7" t="s">
         <v>737</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="N19" s="7" t="s">
         <v>738</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>705</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>706</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="O19" s="7" t="s">
         <v>739</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="P19" s="7" t="s">
         <v>740</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="Q19" s="7" t="s">
         <v>741</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>742</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>743</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>744</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
       <c r="F20" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G20" s="23"/>
       <c r="H20" s="21"/>
@@ -6089,11 +6093,11 @@
       <c r="B21" s="9"/>
       <c r="C21" s="24"/>
       <c r="D21" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="18" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="G21" s="23"/>
       <c r="H21" s="21"/>
@@ -6109,10 +6113,10 @@
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="22">
@@ -6135,10 +6139,10 @@
         <v>45</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
@@ -6148,10 +6152,10 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D23" s="15" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="26"/>
@@ -6166,7 +6170,7 @@
         <v>35</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
@@ -6174,10 +6178,10 @@
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="22">
@@ -6200,23 +6204,23 @@
         <v>20</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
       <c r="R24" s="5" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="22">
@@ -6239,20 +6243,20 @@
         <v>20</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D26" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="22">
@@ -6275,10 +6279,10 @@
         <v>18</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P26" s="21"/>
       <c r="Q26" s="21"/>
@@ -6294,7 +6298,7 @@
       <c r="D28" s="20"/>
       <c r="E28" s="21"/>
       <c r="F28" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="21"/>
@@ -6317,11 +6321,11 @@
     <row r="29" spans="1:18" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" s="24"/>
       <c r="D29" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="18" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="G29" s="23"/>
       <c r="H29" s="21"/>
@@ -6338,10 +6342,10 @@
     <row r="30" spans="1:18" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" s="8"/>
       <c r="D30" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="22">
@@ -6364,26 +6368,26 @@
         <v>128</v>
       </c>
       <c r="N30" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O30" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="21"/>
       <c r="R30" s="9" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="15" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="G31" s="22">
         <v>34</v>
@@ -6401,7 +6405,7 @@
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
       <c r="P31" s="25" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="Q31" s="25">
         <v>1</v>
@@ -6409,10 +6413,10 @@
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="22">
@@ -6435,23 +6439,23 @@
         <v>40</v>
       </c>
       <c r="N32" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O32" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O32" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P32" s="21"/>
       <c r="Q32" s="21"/>
       <c r="R32" s="5" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="33" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="22">
@@ -6474,23 +6478,23 @@
         <v>30</v>
       </c>
       <c r="N33" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O33" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O33" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P33" s="21"/>
       <c r="Q33" s="21"/>
       <c r="R33" s="5" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="34" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="22">
@@ -6513,10 +6517,10 @@
         <v>48</v>
       </c>
       <c r="N34" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O34" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O34" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>
@@ -6526,10 +6530,10 @@
     </row>
     <row r="35" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D35" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="22">
@@ -6552,10 +6556,10 @@
         <v>55</v>
       </c>
       <c r="N35" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P35" s="21"/>
       <c r="Q35" s="21"/>
@@ -6565,10 +6569,10 @@
     </row>
     <row r="36" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="22">
@@ -6591,10 +6595,10 @@
         <v>55</v>
       </c>
       <c r="N36" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O36" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P36" s="21"/>
       <c r="Q36" s="21"/>
@@ -6604,12 +6608,12 @@
     </row>
     <row r="38" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="10" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="21"/>
       <c r="F38" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G38" s="23"/>
       <c r="H38" s="21"/>
@@ -6632,11 +6636,11 @@
     <row r="39" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="24"/>
       <c r="D39" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="18" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="G39" s="23"/>
       <c r="H39" s="21"/>
@@ -6652,10 +6656,10 @@
     </row>
     <row r="40" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D40" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="22">
@@ -6678,26 +6682,26 @@
         <v>128</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O40" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P40" s="21"/>
       <c r="Q40" s="21"/>
       <c r="R40" s="5" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="41" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D41" s="15" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="G41" s="22">
         <v>34</v>
@@ -6715,7 +6719,7 @@
       <c r="N41" s="21"/>
       <c r="O41" s="21"/>
       <c r="P41" s="25" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="Q41" s="25">
         <v>1</v>
@@ -6723,10 +6727,10 @@
     </row>
     <row r="42" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D42" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F42" s="25"/>
       <c r="G42" s="22">
@@ -6749,23 +6753,23 @@
         <v>40</v>
       </c>
       <c r="N42" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O42" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O42" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P42" s="21"/>
       <c r="Q42" s="21"/>
       <c r="R42" s="5" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="43" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D43" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F43" s="25"/>
       <c r="G43" s="22">
@@ -6788,23 +6792,23 @@
         <v>30</v>
       </c>
       <c r="N43" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O43" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O43" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P43" s="21"/>
       <c r="Q43" s="21"/>
       <c r="R43" s="5" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="44" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D44" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="22">
@@ -6827,10 +6831,10 @@
         <v>48</v>
       </c>
       <c r="N44" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O44" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O44" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P44" s="21"/>
       <c r="Q44" s="21"/>
@@ -6840,12 +6844,12 @@
     </row>
     <row r="46" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="10" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
       <c r="F46" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G46" s="23"/>
       <c r="H46" s="21"/>
@@ -6869,11 +6873,11 @@
     <row r="47" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="24"/>
       <c r="D47" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E47" s="21"/>
       <c r="F47" s="18" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="G47" s="23"/>
       <c r="H47" s="21"/>
@@ -6890,10 +6894,10 @@
     </row>
     <row r="48" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D48" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="22">
@@ -6916,10 +6920,10 @@
         <v>55</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O48" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P48" s="21"/>
       <c r="Q48" s="21"/>
@@ -6929,10 +6933,10 @@
     </row>
     <row r="49" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D49" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="22">
@@ -6955,10 +6959,10 @@
         <v>55</v>
       </c>
       <c r="N49" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O49" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P49" s="21"/>
       <c r="Q49" s="21"/>
@@ -6968,12 +6972,12 @@
     </row>
     <row r="51" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" s="10" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="21"/>
       <c r="F51" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G51" s="23"/>
       <c r="H51" s="21"/>
@@ -6996,11 +7000,11 @@
     <row r="52" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="24"/>
       <c r="D52" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E52" s="21"/>
       <c r="F52" s="18" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="G52" s="23"/>
       <c r="H52" s="21"/>
@@ -7016,10 +7020,10 @@
     </row>
     <row r="53" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="22">
@@ -7042,26 +7046,26 @@
         <v>128</v>
       </c>
       <c r="N53" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O53" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P53" s="21"/>
       <c r="Q53" s="21"/>
       <c r="R53" s="5" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="54" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="15" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F54" s="29" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="G54" s="22">
         <v>34</v>
@@ -7079,7 +7083,7 @@
       <c r="N54" s="21"/>
       <c r="O54" s="21"/>
       <c r="P54" s="25" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="Q54" s="25">
         <v>1</v>
@@ -7087,10 +7091,10 @@
     </row>
     <row r="55" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="22">
@@ -7113,23 +7117,23 @@
         <v>40</v>
       </c>
       <c r="N55" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O55" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O55" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P55" s="21"/>
       <c r="Q55" s="21"/>
       <c r="R55" s="5" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="56" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D56" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="22">
@@ -7152,23 +7156,23 @@
         <v>30</v>
       </c>
       <c r="N56" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O56" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O56" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P56" s="21"/>
       <c r="Q56" s="21"/>
       <c r="R56" s="5" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="57" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D57" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F57" s="25"/>
       <c r="G57" s="22">
@@ -7191,10 +7195,10 @@
         <v>48</v>
       </c>
       <c r="N57" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O57" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O57" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P57" s="21"/>
       <c r="Q57" s="21"/>
@@ -7204,12 +7208,12 @@
     </row>
     <row r="59" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C59" s="10" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="21"/>
       <c r="F59" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G59" s="23"/>
       <c r="H59" s="21"/>
@@ -7232,11 +7236,11 @@
     <row r="60" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" s="24"/>
       <c r="D60" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E60" s="21"/>
       <c r="F60" s="18" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="G60" s="23"/>
       <c r="H60" s="21"/>
@@ -7252,10 +7256,10 @@
     </row>
     <row r="61" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D61" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F61" s="25"/>
       <c r="G61" s="22">
@@ -7278,26 +7282,26 @@
         <v>128</v>
       </c>
       <c r="N61" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O61" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P61" s="21"/>
       <c r="Q61" s="21"/>
       <c r="R61" s="5" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="62" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D62" s="15" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F62" s="29" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="G62" s="22">
         <v>34</v>
@@ -7315,7 +7319,7 @@
       <c r="N62" s="21"/>
       <c r="O62" s="21"/>
       <c r="P62" s="25" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="Q62" s="25">
         <v>1</v>
@@ -7323,10 +7327,10 @@
     </row>
     <row r="63" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D63" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F63" s="25"/>
       <c r="G63" s="22">
@@ -7349,23 +7353,23 @@
         <v>40</v>
       </c>
       <c r="N63" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O63" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O63" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P63" s="21"/>
       <c r="Q63" s="21"/>
       <c r="R63" s="5" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="64" spans="3:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D64" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F64" s="25"/>
       <c r="G64" s="22">
@@ -7388,23 +7392,23 @@
         <v>30</v>
       </c>
       <c r="N64" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O64" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O64" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P64" s="21"/>
       <c r="Q64" s="21"/>
       <c r="R64" s="5" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="65" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D65" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F65" s="25"/>
       <c r="G65" s="22">
@@ -7427,10 +7431,10 @@
         <v>48</v>
       </c>
       <c r="N65" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O65" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O65" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P65" s="21"/>
       <c r="Q65" s="21"/>
@@ -7454,7 +7458,7 @@
       <c r="D67" s="20"/>
       <c r="E67" s="21"/>
       <c r="F67" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G67" s="23"/>
       <c r="H67" s="21"/>
@@ -7480,11 +7484,11 @@
       <c r="B68" s="30"/>
       <c r="C68" s="24"/>
       <c r="D68" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E68" s="21"/>
       <c r="F68" s="18" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="G68" s="23"/>
       <c r="H68" s="21"/>
@@ -7504,10 +7508,10 @@
       <c r="B69" s="30"/>
       <c r="C69" s="8"/>
       <c r="D69" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="F69" s="25"/>
       <c r="G69" s="22">
@@ -7530,10 +7534,10 @@
         <v>45</v>
       </c>
       <c r="N69" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O69" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P69" s="21"/>
       <c r="Q69" s="21"/>
@@ -7546,10 +7550,10 @@
       <c r="B70" s="30"/>
       <c r="C70" s="8"/>
       <c r="D70" s="15" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="26"/>
@@ -7564,7 +7568,7 @@
         <v>35</v>
       </c>
       <c r="N70" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O70" s="21"/>
       <c r="P70" s="21"/>
@@ -7578,10 +7582,10 @@
       <c r="B71" s="30"/>
       <c r="C71" s="8"/>
       <c r="D71" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="F71" s="25"/>
       <c r="G71" s="22">
@@ -7604,15 +7608,15 @@
         <v>20</v>
       </c>
       <c r="N71" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O71" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P71" s="21"/>
       <c r="Q71" s="21"/>
       <c r="R71" s="5" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="72" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7620,10 +7624,10 @@
       <c r="B72" s="30"/>
       <c r="C72" s="8"/>
       <c r="D72" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="F72" s="25"/>
       <c r="G72" s="22">
@@ -7646,10 +7650,10 @@
         <v>20</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O72" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P72" s="21"/>
       <c r="Q72" s="21"/>
@@ -7660,10 +7664,10 @@
       <c r="B73" s="30"/>
       <c r="C73" s="8"/>
       <c r="D73" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="F73" s="25"/>
       <c r="G73" s="22">
@@ -7686,10 +7690,10 @@
         <v>18</v>
       </c>
       <c r="N73" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O73" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P73" s="21"/>
       <c r="Q73" s="21"/>
@@ -7700,10 +7704,10 @@
       <c r="B74" s="30"/>
       <c r="C74" s="30"/>
       <c r="D74" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F74" s="25"/>
       <c r="G74" s="22">
@@ -7726,15 +7730,15 @@
         <v>128</v>
       </c>
       <c r="N74" s="25" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="O74" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P74" s="21"/>
       <c r="Q74" s="21"/>
       <c r="R74" s="5" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="75" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7742,10 +7746,10 @@
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
       <c r="D75" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="22">
@@ -7768,15 +7772,15 @@
         <v>45</v>
       </c>
       <c r="N75" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O75" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O75" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P75" s="21"/>
       <c r="Q75" s="21"/>
       <c r="R75" s="5" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="76" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7784,10 +7788,10 @@
       <c r="B76" s="30"/>
       <c r="C76" s="30"/>
       <c r="D76" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F76" s="25"/>
       <c r="G76" s="22">
@@ -7810,15 +7814,15 @@
         <v>35</v>
       </c>
       <c r="N76" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O76" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O76" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P76" s="21"/>
       <c r="Q76" s="21"/>
       <c r="R76" s="5" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="77" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7832,12 +7836,12 @@
       <c r="A78" s="30"/>
       <c r="B78" s="30"/>
       <c r="C78" s="10" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D78" s="20"/>
       <c r="E78" s="21"/>
       <c r="F78" s="22" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="G78" s="23"/>
       <c r="H78" s="21"/>
@@ -7863,11 +7867,11 @@
       <c r="B79" s="30"/>
       <c r="C79" s="24"/>
       <c r="D79" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E79" s="21"/>
       <c r="F79" s="18" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="G79" s="23"/>
       <c r="H79" s="21"/>
@@ -7887,10 +7891,10 @@
       <c r="B80" s="30"/>
       <c r="C80" s="8"/>
       <c r="D80" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="F80" s="25"/>
       <c r="G80" s="22">
@@ -7913,10 +7917,10 @@
         <v>35</v>
       </c>
       <c r="N80" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O80" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P80" s="21"/>
       <c r="Q80" s="21"/>
@@ -7929,10 +7933,10 @@
       <c r="B81" s="30"/>
       <c r="C81" s="8"/>
       <c r="D81" s="15" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="F81" s="21"/>
       <c r="G81" s="26"/>
@@ -7947,7 +7951,7 @@
         <v>30</v>
       </c>
       <c r="N81" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O81" s="21"/>
       <c r="P81" s="21"/>
@@ -7961,10 +7965,10 @@
       <c r="B82" s="30"/>
       <c r="C82" s="8"/>
       <c r="D82" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="F82" s="25"/>
       <c r="G82" s="22">
@@ -7987,15 +7991,15 @@
         <v>20</v>
       </c>
       <c r="N82" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O82" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P82" s="21"/>
       <c r="Q82" s="21"/>
       <c r="R82" s="5" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="83" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -8003,10 +8007,10 @@
       <c r="B83" s="30"/>
       <c r="C83" s="8"/>
       <c r="D83" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="F83" s="25"/>
       <c r="G83" s="22">
@@ -8029,10 +8033,10 @@
         <v>20</v>
       </c>
       <c r="N83" s="25" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="O83" s="25" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="P83" s="21"/>
       <c r="Q83" s="21"/>
@@ -8043,10 +8047,10 @@
       <c r="B84" s="30"/>
       <c r="C84" s="8"/>
       <c r="D84" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="F84" s="25"/>
       <c r="G84" s="22">
@@ -8069,10 +8073,10 @@
         <v>18</v>
       </c>
       <c r="N84" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="O84" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P84" s="21"/>
       <c r="Q84" s="21"/>
@@ -8083,10 +8087,10 @@
       <c r="B85" s="30"/>
       <c r="C85" s="30"/>
       <c r="D85" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F85" s="25"/>
       <c r="G85" s="22">
@@ -8109,15 +8113,15 @@
         <v>128</v>
       </c>
       <c r="N85" s="25" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="O85" s="25" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="P85" s="21"/>
       <c r="Q85" s="21"/>
       <c r="R85" s="5" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="86" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -8125,13 +8129,13 @@
       <c r="B86" s="30"/>
       <c r="C86" s="30"/>
       <c r="D86" s="15" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F86" s="29" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="G86" s="22">
         <v>0</v>
@@ -8149,7 +8153,7 @@
       <c r="N86" s="21"/>
       <c r="O86" s="21"/>
       <c r="P86" s="25" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="Q86" s="25">
         <v>1</v>
@@ -8161,10 +8165,10 @@
       <c r="B87" s="30"/>
       <c r="C87" s="30"/>
       <c r="D87" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F87" s="25"/>
       <c r="G87" s="22">
@@ -8187,15 +8191,15 @@
         <v>45</v>
       </c>
       <c r="N87" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O87" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O87" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P87" s="21"/>
       <c r="Q87" s="21"/>
       <c r="R87" s="5" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="88" spans="1:18" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -8203,10 +8207,10 @@
       <c r="B88" s="30"/>
       <c r="C88" s="30"/>
       <c r="D88" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F88" s="25"/>
       <c r="G88" s="22">
@@ -8229,20 +8233,20 @@
         <v>30</v>
       </c>
       <c r="N88" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="O88" s="25" t="s">
         <v>751</v>
-      </c>
-      <c r="O88" s="25" t="s">
-        <v>755</v>
       </c>
       <c r="P88" s="21"/>
       <c r="Q88" s="21"/>
       <c r="R88" s="5" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C90" s="10" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="21"/>
@@ -8268,11 +8272,11 @@
     <row r="91" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C91" s="24"/>
       <c r="D91" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E91" s="21"/>
       <c r="F91" s="18" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="G91" s="23"/>
       <c r="H91" s="21"/>
@@ -8288,7 +8292,7 @@
     </row>
     <row r="93" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C93" s="10" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D93" s="20"/>
       <c r="E93" s="21"/>
@@ -8314,11 +8318,11 @@
     <row r="94" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C94" s="24"/>
       <c r="D94" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E94" s="21"/>
       <c r="F94" s="18" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="G94" s="23"/>
       <c r="H94" s="21"/>
@@ -8334,7 +8338,7 @@
     </row>
     <row r="96" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C96" s="10" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D96" s="20"/>
       <c r="E96" s="21"/>
@@ -8360,11 +8364,11 @@
     <row r="97" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C97" s="24"/>
       <c r="D97" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E97" s="21"/>
       <c r="F97" s="18" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="G97" s="23"/>
       <c r="H97" s="21"/>
@@ -8380,7 +8384,7 @@
     </row>
     <row r="99" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C99" s="10" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D99" s="20"/>
       <c r="E99" s="21"/>
@@ -8406,11 +8410,11 @@
     <row r="100" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C100" s="24"/>
       <c r="D100" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E100" s="21"/>
       <c r="F100" s="18" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="G100" s="23"/>
       <c r="H100" s="21"/>
@@ -8426,7 +8430,7 @@
     </row>
     <row r="102" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C102" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="D102" s="20"/>
       <c r="E102" s="21"/>
@@ -8452,11 +8456,11 @@
     <row r="103" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C103" s="24"/>
       <c r="D103" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E103" s="21"/>
       <c r="F103" s="18" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="G103" s="23"/>
       <c r="H103" s="21"/>
@@ -8472,7 +8476,7 @@
     </row>
     <row r="105" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C105" s="10" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D105" s="20"/>
       <c r="E105" s="21"/>
@@ -8498,11 +8502,11 @@
     <row r="106" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C106" s="24"/>
       <c r="D106" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E106" s="21"/>
       <c r="F106" s="18" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="G106" s="23"/>
       <c r="H106" s="21"/>
@@ -8518,7 +8522,7 @@
     </row>
     <row r="108" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C108" s="10" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="D108" s="20"/>
       <c r="E108" s="21"/>
@@ -8544,11 +8548,11 @@
     <row r="109" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C109" s="24"/>
       <c r="D109" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E109" s="21"/>
       <c r="F109" s="18" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="G109" s="23"/>
       <c r="H109" s="21"/>
@@ -8564,7 +8568,7 @@
     </row>
     <row r="111" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C111" s="10" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D111" s="20"/>
       <c r="E111" s="21"/>
@@ -8590,11 +8594,11 @@
     <row r="112" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C112" s="24"/>
       <c r="D112" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E112" s="21"/>
       <c r="F112" s="18" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="G112" s="23"/>
       <c r="H112" s="21"/>
@@ -8610,7 +8614,7 @@
     </row>
     <row r="114" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C114" s="10" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="D114" s="20"/>
       <c r="E114" s="21"/>
@@ -8636,11 +8640,11 @@
     <row r="115" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C115" s="24"/>
       <c r="D115" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E115" s="21"/>
       <c r="F115" s="18" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="G115" s="23"/>
       <c r="H115" s="21"/>
@@ -8656,7 +8660,7 @@
     </row>
     <row r="117" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C117" s="10" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D117" s="20"/>
       <c r="E117" s="21"/>
@@ -8682,11 +8686,11 @@
     <row r="118" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C118" s="24"/>
       <c r="D118" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E118" s="21"/>
       <c r="F118" s="18" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="G118" s="23"/>
       <c r="H118" s="21"/>
@@ -8702,7 +8706,7 @@
     </row>
     <row r="120" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C120" s="10" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="D120" s="20"/>
       <c r="E120" s="21"/>
@@ -8728,11 +8732,11 @@
     <row r="121" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C121" s="24"/>
       <c r="D121" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E121" s="21"/>
       <c r="F121" s="18" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="G121" s="23"/>
       <c r="H121" s="21"/>
@@ -8748,7 +8752,7 @@
     </row>
     <row r="123" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C123" s="10" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D123" s="20"/>
       <c r="E123" s="21"/>
@@ -8774,11 +8778,11 @@
     <row r="124" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C124" s="24"/>
       <c r="D124" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E124" s="21"/>
       <c r="F124" s="18" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="G124" s="23"/>
       <c r="H124" s="21"/>
@@ -8794,7 +8798,7 @@
     </row>
     <row r="126" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C126" s="10" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D126" s="20"/>
       <c r="E126" s="21"/>
@@ -8820,11 +8824,11 @@
     <row r="127" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C127" s="24"/>
       <c r="D127" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E127" s="21"/>
       <c r="F127" s="18" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="G127" s="23"/>
       <c r="H127" s="21"/>
@@ -8840,7 +8844,7 @@
     </row>
     <row r="129" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C129" s="10" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D129" s="20"/>
       <c r="E129" s="21"/>
@@ -8866,11 +8870,11 @@
     <row r="130" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C130" s="24"/>
       <c r="D130" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E130" s="21"/>
       <c r="F130" s="18" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="G130" s="23"/>
       <c r="H130" s="21"/>
@@ -8886,7 +8890,7 @@
     </row>
     <row r="132" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C132" s="10" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="D132" s="20"/>
       <c r="E132" s="21"/>
@@ -8912,11 +8916,11 @@
     <row r="133" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C133" s="24"/>
       <c r="D133" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E133" s="21"/>
       <c r="F133" s="18" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="G133" s="23"/>
       <c r="H133" s="21"/>
@@ -8932,7 +8936,7 @@
     </row>
     <row r="135" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C135" s="10" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D135" s="20"/>
       <c r="E135" s="21"/>
@@ -8958,11 +8962,11 @@
     <row r="136" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C136" s="24"/>
       <c r="D136" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E136" s="21"/>
       <c r="F136" s="18" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="G136" s="23"/>
       <c r="H136" s="21"/>
@@ -8978,7 +8982,7 @@
     </row>
     <row r="138" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C138" s="10" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="D138" s="20"/>
       <c r="E138" s="21"/>
@@ -9004,11 +9008,11 @@
     <row r="139" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C139" s="24"/>
       <c r="D139" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E139" s="21"/>
       <c r="F139" s="18" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="G139" s="23"/>
       <c r="H139" s="21"/>
@@ -9024,7 +9028,7 @@
     </row>
     <row r="141" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C141" s="10" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D141" s="20"/>
       <c r="E141" s="21"/>
@@ -9050,11 +9054,11 @@
     <row r="142" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C142" s="24"/>
       <c r="D142" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E142" s="21"/>
       <c r="F142" s="18" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="G142" s="23"/>
       <c r="H142" s="21"/>
@@ -9070,7 +9074,7 @@
     </row>
     <row r="144" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C144" s="10" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="D144" s="20"/>
       <c r="E144" s="21"/>
@@ -9096,11 +9100,11 @@
     <row r="145" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C145" s="24"/>
       <c r="D145" s="15" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E145" s="21"/>
       <c r="F145" s="18" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="G145" s="23"/>
       <c r="H145" s="21"/>
@@ -9116,7 +9120,7 @@
     </row>
     <row r="147" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C147" s="10" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="D147" s="20"/>
       <c r="E147" s="21"/>
@@ -9142,7 +9146,7 @@
     <row r="148" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C148" s="24"/>
       <c r="D148" s="15" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="E148" s="18" t="s">
         <v>635</v>
@@ -9162,10 +9166,10 @@
     </row>
     <row r="149" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D149" s="15" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="E149" s="18" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="F149" s="23"/>
       <c r="G149" s="23"/>
@@ -9181,6 +9185,9 @@
       <c r="Q149" s="21"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>